<commit_message>
Fix heat rate modeling syntax
</commit_message>
<xml_diff>
--- a/model/Output Files/Year 0.xlsx
+++ b/model/Output Files/Year 0.xlsx
@@ -530,7 +530,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>2.884000000000027</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -1125,19 +1125,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>76376.03999999999</v>
+        <v>76271.06239999995</v>
       </c>
       <c r="C2" t="n">
         <v>58600</v>
       </c>
       <c r="D2" t="n">
-        <v>9410.572794921793</v>
+        <v>9300.638068405267</v>
       </c>
       <c r="E2" t="n">
         <v>10370</v>
       </c>
       <c r="F2" t="n">
-        <v>-2004.53279492179</v>
+        <v>-1999.575668405316</v>
       </c>
     </row>
   </sheetData>
@@ -1406,7 +1406,7 @@
         <v>20.8</v>
       </c>
       <c r="H2" t="n">
-        <v>41.6</v>
+        <v>40.03636363636365</v>
       </c>
       <c r="I2" t="n">
         <v>52</v>
@@ -1418,7 +1418,7 @@
         <v>72.8</v>
       </c>
       <c r="L2" t="n">
-        <v>81.63636363636365</v>
+        <v>83.2</v>
       </c>
       <c r="M2" t="n">
         <v>93.59999999999999</v>
@@ -1486,7 +1486,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>41.6</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
         <v>62.4</v>
@@ -1495,10 +1495,10 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>93.59999999999999</v>
       </c>
       <c r="M3" t="n">
-        <v>104</v>
+        <v>42.2531170288747</v>
       </c>
       <c r="N3" t="n">
         <v>83.2</v>
@@ -1510,10 +1510,10 @@
         <v>52</v>
       </c>
       <c r="Q3" t="n">
-        <v>47.45311702887471</v>
+        <v>26</v>
       </c>
       <c r="R3" t="n">
-        <v>0</v>
+        <v>31.2</v>
       </c>
       <c r="S3" t="n">
         <v>20.8</v>
@@ -1572,19 +1572,19 @@
         <v>41.6</v>
       </c>
       <c r="L4" t="n">
+        <v>29.58312417100293</v>
+      </c>
+      <c r="M4" t="n">
+        <v>83.2</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
         <v>72.8</v>
       </c>
-      <c r="M4" t="n">
-        <v>23.4</v>
-      </c>
-      <c r="N4" t="n">
-        <v>83.2</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0</v>
-      </c>
       <c r="P4" t="n">
-        <v>6.183124171003051</v>
+        <v>0</v>
       </c>
       <c r="Q4" t="n">
         <v>20.8</v>
@@ -1730,7 +1730,7 @@
         <v>13</v>
       </c>
       <c r="H2" t="n">
-        <v>28.6</v>
+        <v>27.03636363636365</v>
       </c>
       <c r="I2" t="n">
         <v>20.8</v>
@@ -1742,7 +1742,7 @@
         <v>46.8</v>
       </c>
       <c r="L2" t="n">
-        <v>60.83636363636364</v>
+        <v>62.4</v>
       </c>
       <c r="M2" t="n">
         <v>70.2</v>
@@ -1810,7 +1810,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>41.6</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
         <v>62.4</v>
@@ -1819,10 +1819,10 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>93.59999999999999</v>
       </c>
       <c r="M3" t="n">
-        <v>80.59999999999999</v>
+        <v>18.8531170288747</v>
       </c>
       <c r="N3" t="n">
         <v>57.2</v>
@@ -1834,10 +1834,10 @@
         <v>23.4</v>
       </c>
       <c r="Q3" t="n">
-        <v>21.45311702887471</v>
+        <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>0</v>
+        <v>31.2</v>
       </c>
       <c r="S3" t="n">
         <v>0</v>
@@ -1896,19 +1896,19 @@
         <v>41.6</v>
       </c>
       <c r="L4" t="n">
+        <v>29.58312417100293</v>
+      </c>
+      <c r="M4" t="n">
+        <v>59.8</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
         <v>72.8</v>
       </c>
-      <c r="M4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" t="n">
-        <v>83.2</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0</v>
-      </c>
       <c r="P4" t="n">
-        <v>6.18312417100305</v>
+        <v>0</v>
       </c>
       <c r="Q4" t="n">
         <v>20.8</v>
@@ -2042,7 +2042,7 @@
         <v>19.5</v>
       </c>
       <c r="D2" t="n">
-        <v>10.11599999999997</v>
+        <v>13</v>
       </c>
       <c r="E2" t="n">
         <v>13</v>
@@ -2087,7 +2087,7 @@
         <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>10.4</v>
+        <v>7.516000000000011</v>
       </c>
       <c r="T2" t="n">
         <v>31.2</v>
@@ -2360,16 +2360,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>185.7777777777778</v>
+        <v>188.6909090909091</v>
       </c>
       <c r="C2" t="n">
-        <v>166.0808080808081</v>
+        <v>168.9939393939394</v>
       </c>
       <c r="D2" t="n">
-        <v>155.8626262626263</v>
+        <v>155.8626262626262</v>
       </c>
       <c r="E2" t="n">
-        <v>142.7313131313132</v>
+        <v>142.7313131313131</v>
       </c>
       <c r="F2" t="n">
         <v>129.6</v>
@@ -2378,16 +2378,16 @@
         <v>142.47</v>
       </c>
       <c r="H2" t="n">
-        <v>170.784</v>
+        <v>169.236</v>
       </c>
       <c r="I2" t="n">
-        <v>191.376</v>
+        <v>189.828</v>
       </c>
       <c r="J2" t="n">
-        <v>214.542</v>
+        <v>212.994</v>
       </c>
       <c r="K2" t="n">
-        <v>260.874</v>
+        <v>259.326</v>
       </c>
       <c r="L2" t="n">
         <v>321.102</v>
@@ -2411,25 +2411,25 @@
         <v>648</v>
       </c>
       <c r="S2" t="n">
-        <v>637.4949494949495</v>
+        <v>640.4080808080807</v>
       </c>
       <c r="T2" t="n">
-        <v>605.979797979798</v>
+        <v>608.8929292929292</v>
       </c>
       <c r="U2" t="n">
-        <v>487.7979797979798</v>
+        <v>490.7111111111111</v>
       </c>
       <c r="V2" t="n">
-        <v>389.3131313131314</v>
+        <v>392.2262626262626</v>
       </c>
       <c r="W2" t="n">
-        <v>310.5252525252525</v>
+        <v>313.4383838383839</v>
       </c>
       <c r="X2" t="n">
-        <v>258</v>
+        <v>260.9131313131313</v>
       </c>
       <c r="Y2" t="n">
-        <v>218.6060606060606</v>
+        <v>221.5191919191919</v>
       </c>
     </row>
     <row r="3">
@@ -2458,31 +2458,31 @@
         <v>129.6</v>
       </c>
       <c r="I3" t="n">
-        <v>170.784</v>
+        <v>129.6</v>
       </c>
       <c r="J3" t="n">
-        <v>232.56</v>
+        <v>191.376</v>
       </c>
       <c r="K3" t="n">
-        <v>232.56</v>
+        <v>191.376</v>
       </c>
       <c r="L3" t="n">
-        <v>232.56</v>
+        <v>284.04</v>
       </c>
       <c r="M3" t="n">
-        <v>312.354</v>
+        <v>302.704585858586</v>
       </c>
       <c r="N3" t="n">
-        <v>368.982</v>
+        <v>359.332585858586</v>
       </c>
       <c r="O3" t="n">
-        <v>441.054</v>
+        <v>431.404585858586</v>
       </c>
       <c r="P3" t="n">
-        <v>464.22</v>
+        <v>454.570585858586</v>
       </c>
       <c r="Q3" t="n">
-        <v>485.4585858585859</v>
+        <v>454.570585858586</v>
       </c>
       <c r="R3" t="n">
         <v>485.4585858585859</v>
@@ -2514,76 +2514,76 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>168.9939393939394</v>
+        <v>444.4646464646465</v>
       </c>
       <c r="C4" t="n">
-        <v>149.2969696969697</v>
+        <v>424.7676767676768</v>
       </c>
       <c r="D4" t="n">
-        <v>149.2969696969697</v>
+        <v>424.7676767676768</v>
       </c>
       <c r="E4" t="n">
-        <v>149.2969696969697</v>
+        <v>424.7676767676768</v>
       </c>
       <c r="F4" t="n">
-        <v>149.2969696969697</v>
+        <v>424.7676767676768</v>
       </c>
       <c r="G4" t="n">
-        <v>129.6</v>
+        <v>405.0707070707071</v>
       </c>
       <c r="H4" t="n">
-        <v>129.6</v>
+        <v>405.0707070707071</v>
       </c>
       <c r="I4" t="n">
-        <v>129.6</v>
+        <v>405.0707070707071</v>
       </c>
       <c r="J4" t="n">
-        <v>139.896</v>
+        <v>415.3667070707071</v>
       </c>
       <c r="K4" t="n">
-        <v>181.08</v>
+        <v>456.5507070707071</v>
       </c>
       <c r="L4" t="n">
-        <v>253.152</v>
+        <v>485.838</v>
       </c>
       <c r="M4" t="n">
-        <v>253.152</v>
+        <v>545.04</v>
       </c>
       <c r="N4" t="n">
-        <v>335.52</v>
+        <v>545.04</v>
       </c>
       <c r="O4" t="n">
-        <v>335.52</v>
+        <v>617.112</v>
       </c>
       <c r="P4" t="n">
-        <v>341.641292929293</v>
+        <v>617.112</v>
       </c>
       <c r="Q4" t="n">
-        <v>362.233292929293</v>
+        <v>637.704</v>
       </c>
       <c r="R4" t="n">
-        <v>372.529292929293</v>
+        <v>648</v>
       </c>
       <c r="S4" t="n">
-        <v>372.529292929293</v>
+        <v>648</v>
       </c>
       <c r="T4" t="n">
-        <v>241.2161616161616</v>
+        <v>516.6868686868687</v>
       </c>
       <c r="U4" t="n">
-        <v>241.2161616161616</v>
+        <v>516.6868686868687</v>
       </c>
       <c r="V4" t="n">
-        <v>241.2161616161616</v>
+        <v>516.6868686868687</v>
       </c>
       <c r="W4" t="n">
-        <v>241.2161616161616</v>
+        <v>516.6868686868687</v>
       </c>
       <c r="X4" t="n">
-        <v>241.2161616161616</v>
+        <v>516.6868686868687</v>
       </c>
       <c r="Y4" t="n">
-        <v>201.8222222222222</v>
+        <v>477.2929292929293</v>
       </c>
     </row>
   </sheetData>
@@ -3383,7 +3383,7 @@
         <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>0</v>
+        <v>2.883999999999991</v>
       </c>
       <c r="T2" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Clean up code and fix output
</commit_message>
<xml_diff>
--- a/model/Output Files/Year 0.xlsx
+++ b/model/Output Files/Year 0.xlsx
@@ -20,6 +20,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Costs and Revenues" sheetId="11" state="visible" r:id="rId11"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Capacities" sheetId="12" state="visible" r:id="rId12"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Connected Households" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Yearly demand" sheetId="14" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1295,6 +1296,330 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Y4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>-32.5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-19.5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-13</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-13</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-13</v>
+      </c>
+      <c r="G2" t="n">
+        <v>142.5</v>
+      </c>
+      <c r="H2" t="n">
+        <v>291.5</v>
+      </c>
+      <c r="I2" t="n">
+        <v>327</v>
+      </c>
+      <c r="J2" t="n">
+        <v>388.5</v>
+      </c>
+      <c r="K2" t="n">
+        <v>502</v>
+      </c>
+      <c r="L2" t="n">
+        <v>596</v>
+      </c>
+      <c r="M2" t="n">
+        <v>670.5</v>
+      </c>
+      <c r="N2" t="n">
+        <v>745</v>
+      </c>
+      <c r="O2" t="n">
+        <v>651</v>
+      </c>
+      <c r="P2" t="n">
+        <v>576.5</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>502</v>
+      </c>
+      <c r="R2" t="n">
+        <v>320.5</v>
+      </c>
+      <c r="S2" t="n">
+        <v>139</v>
+      </c>
+      <c r="T2" t="n">
+        <v>32</v>
+      </c>
+      <c r="U2" t="n">
+        <v>-117</v>
+      </c>
+      <c r="V2" t="n">
+        <v>-97.5</v>
+      </c>
+      <c r="W2" t="n">
+        <v>-78</v>
+      </c>
+      <c r="X2" t="n">
+        <v>-52</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>-39</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>-32.5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-19.5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-13</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>-19.5</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>324</v>
+      </c>
+      <c r="J3" t="n">
+        <v>486</v>
+      </c>
+      <c r="K3" t="n">
+        <v>648</v>
+      </c>
+      <c r="L3" t="n">
+        <v>729</v>
+      </c>
+      <c r="M3" t="n">
+        <v>751.5</v>
+      </c>
+      <c r="N3" t="n">
+        <v>583</v>
+      </c>
+      <c r="O3" t="n">
+        <v>567</v>
+      </c>
+      <c r="P3" t="n">
+        <v>333.5</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>340</v>
+      </c>
+      <c r="R3" t="n">
+        <v>243</v>
+      </c>
+      <c r="S3" t="n">
+        <v>57.99999999999999</v>
+      </c>
+      <c r="T3" t="n">
+        <v>-130</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" t="n">
+        <v>-78</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>-39</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>-32.5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-19.5</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-19.5</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>81</v>
+      </c>
+      <c r="K4" t="n">
+        <v>324</v>
+      </c>
+      <c r="L4" t="n">
+        <v>567</v>
+      </c>
+      <c r="M4" t="n">
+        <v>589.5</v>
+      </c>
+      <c r="N4" t="n">
+        <v>648</v>
+      </c>
+      <c r="O4" t="n">
+        <v>567</v>
+      </c>
+      <c r="P4" t="n">
+        <v>324</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>162</v>
+      </c>
+      <c r="R4" t="n">
+        <v>81</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>-130</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>-39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Set for test case
</commit_message>
<xml_diff>
--- a/model/Output Files/Year 0.xlsx
+++ b/model/Output Files/Year 0.xlsx
@@ -1126,19 +1126,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>77388.66797673708</v>
+        <v>77388.66797673714</v>
       </c>
       <c r="C2" t="n">
-        <v>28000</v>
+        <v>45400</v>
       </c>
       <c r="D2" t="n">
-        <v>7066.221906540152</v>
+        <v>9992.976702785445</v>
       </c>
       <c r="E2" t="n">
-        <v>8900</v>
+        <v>9770</v>
       </c>
       <c r="F2" t="n">
-        <v>33422.44607019693</v>
+        <v>12225.69127395169</v>
       </c>
     </row>
   </sheetData>
@@ -1200,10 +1200,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="C3" t="n">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -1728,46 +1728,46 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>13.6</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>27.2</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>40.8</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>47.6</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>54.4</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>61.2</v>
       </c>
       <c r="N2" t="n">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>61.2</v>
       </c>
       <c r="P2" t="n">
-        <v>0</v>
+        <v>54.4</v>
       </c>
       <c r="Q2" t="n">
-        <v>0</v>
+        <v>47.6</v>
       </c>
       <c r="R2" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="S2" t="n">
-        <v>0</v>
+        <v>20.4</v>
       </c>
       <c r="T2" t="n">
-        <v>0</v>
+        <v>13.6</v>
       </c>
       <c r="U2" t="n">
         <v>0</v>
@@ -1811,37 +1811,37 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>27.2</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>40.8</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>54.4</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>61.2</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>54.4</v>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>47.6</v>
       </c>
       <c r="P3" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="Q3" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="R3" t="n">
-        <v>0</v>
+        <v>20.4</v>
       </c>
       <c r="S3" t="n">
-        <v>0</v>
+        <v>13.6</v>
       </c>
       <c r="T3" t="n">
         <v>0</v>
@@ -1891,31 +1891,31 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>6.8</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>27.2</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>47.6</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>54.4</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>37.5831241710018</v>
       </c>
       <c r="O4" t="n">
-        <v>0</v>
+        <v>47.6</v>
       </c>
       <c r="P4" t="n">
-        <v>0</v>
+        <v>27.2</v>
       </c>
       <c r="Q4" t="n">
-        <v>0</v>
+        <v>13.6</v>
       </c>
       <c r="R4" t="n">
-        <v>0</v>
+        <v>6.8</v>
       </c>
       <c r="S4" t="n">
         <v>0</v>
@@ -2052,43 +2052,43 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>50.7</v>
+        <v>64.3</v>
       </c>
       <c r="H2" t="n">
-        <v>26.5</v>
+        <v>53.7</v>
       </c>
       <c r="I2" t="n">
-        <v>150</v>
+        <v>51.6</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>21.6</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>33.6</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>37.8</v>
       </c>
       <c r="N2" t="n">
-        <v>150</v>
+        <v>42</v>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="P2" t="n">
-        <v>0</v>
+        <v>25.8</v>
       </c>
       <c r="Q2" t="n">
-        <v>92.0342720130611</v>
+        <v>21.6</v>
       </c>
       <c r="R2" t="n">
-        <v>14.9</v>
+        <v>48.9</v>
       </c>
       <c r="S2" t="n">
-        <v>0</v>
+        <v>51.43427201306103</v>
       </c>
       <c r="T2" t="n">
         <v>0</v>
@@ -2135,34 +2135,34 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>150</v>
+        <v>27.2</v>
       </c>
       <c r="J3" t="n">
-        <v>8.230792776247702</v>
+        <v>40.8</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>54.4</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>61.2</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>44.6</v>
       </c>
       <c r="N3" t="n">
-        <v>150</v>
+        <v>28.63079277624804</v>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>47.6</v>
       </c>
       <c r="P3" t="n">
-        <v>0</v>
+        <v>5.4</v>
       </c>
       <c r="Q3" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R3" t="n">
-        <v>30</v>
+        <v>20.4</v>
       </c>
       <c r="S3" t="n">
         <v>0</v>
@@ -2215,31 +2215,31 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>10</v>
+        <v>6.8</v>
       </c>
       <c r="K4" t="n">
-        <v>125.3831241710019</v>
+        <v>27.2</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>47.6</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>37.5831241710018</v>
       </c>
       <c r="O4" t="n">
-        <v>0</v>
+        <v>47.6</v>
       </c>
       <c r="P4" t="n">
-        <v>40</v>
+        <v>27.2</v>
       </c>
       <c r="Q4" t="n">
-        <v>60</v>
+        <v>13.6</v>
       </c>
       <c r="R4" t="n">
-        <v>10</v>
+        <v>6.8</v>
       </c>
       <c r="S4" t="n">
         <v>0</v>
@@ -2700,40 +2700,40 @@
         <v>120</v>
       </c>
       <c r="G2" t="n">
-        <v>170.193</v>
+        <v>183.657</v>
       </c>
       <c r="H2" t="n">
-        <v>196.428</v>
+        <v>236.82</v>
       </c>
       <c r="I2" t="n">
-        <v>344.928</v>
+        <v>287.904</v>
       </c>
       <c r="J2" t="n">
-        <v>344.928</v>
+        <v>289.686</v>
       </c>
       <c r="K2" t="n">
-        <v>344.928</v>
+        <v>311.07</v>
       </c>
       <c r="L2" t="n">
-        <v>344.928</v>
+        <v>344.334</v>
       </c>
       <c r="M2" t="n">
-        <v>344.928</v>
+        <v>381.756</v>
       </c>
       <c r="N2" t="n">
-        <v>493.428</v>
+        <v>423.336</v>
       </c>
       <c r="O2" t="n">
-        <v>493.428</v>
+        <v>453.0359999999999</v>
       </c>
       <c r="P2" t="n">
-        <v>493.428</v>
+        <v>478.578</v>
       </c>
       <c r="Q2" t="n">
-        <v>584.5419292929305</v>
+        <v>499.962</v>
       </c>
       <c r="R2" t="n">
-        <v>599.2929292929305</v>
+        <v>548.373</v>
       </c>
       <c r="S2" t="n">
         <v>599.2929292929305</v>
@@ -2765,7 +2765,7 @@
         <v>172.5252525252518</v>
       </c>
       <c r="C3" t="n">
-        <v>152.8282828282828</v>
+        <v>152.8282828282829</v>
       </c>
       <c r="D3" t="n">
         <v>139.6969696969689</v>
@@ -2783,31 +2783,31 @@
         <v>120</v>
       </c>
       <c r="I3" t="n">
-        <v>268.5</v>
+        <v>146.928</v>
       </c>
       <c r="J3" t="n">
-        <v>276.6484848484852</v>
+        <v>187.32</v>
       </c>
       <c r="K3" t="n">
-        <v>276.6484848484852</v>
+        <v>241.176</v>
       </c>
       <c r="L3" t="n">
-        <v>276.6484848484852</v>
+        <v>301.764</v>
       </c>
       <c r="M3" t="n">
-        <v>276.6484848484852</v>
+        <v>345.918</v>
       </c>
       <c r="N3" t="n">
-        <v>425.1484848484852</v>
+        <v>374.2624848484855</v>
       </c>
       <c r="O3" t="n">
-        <v>425.1484848484852</v>
+        <v>421.3864848484856</v>
       </c>
       <c r="P3" t="n">
-        <v>425.1484848484852</v>
+        <v>426.7324848484852</v>
       </c>
       <c r="Q3" t="n">
-        <v>425.1484848484852</v>
+        <v>434.6524848484852</v>
       </c>
       <c r="R3" t="n">
         <v>454.8484848484852</v>
@@ -2863,28 +2863,28 @@
         <v>120</v>
       </c>
       <c r="J4" t="n">
-        <v>129.9</v>
+        <v>126.732</v>
       </c>
       <c r="K4" t="n">
-        <v>254.0292929292919</v>
+        <v>153.66</v>
       </c>
       <c r="L4" t="n">
-        <v>254.0292929292919</v>
+        <v>200.784</v>
       </c>
       <c r="M4" t="n">
-        <v>254.0292929292919</v>
+        <v>231.474</v>
       </c>
       <c r="N4" t="n">
-        <v>254.0292929292919</v>
+        <v>268.6812929292918</v>
       </c>
       <c r="O4" t="n">
-        <v>254.0292929292919</v>
+        <v>315.8052929292918</v>
       </c>
       <c r="P4" t="n">
-        <v>293.6292929292919</v>
+        <v>342.7332929292918</v>
       </c>
       <c r="Q4" t="n">
-        <v>353.0292929292918</v>
+        <v>356.1972929292918</v>
       </c>
       <c r="R4" t="n">
         <v>362.9292929292918</v>
@@ -3354,7 +3354,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>37.2</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
@@ -3387,7 +3387,7 @@
         <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U2" t="n">
         <v>0</v>
@@ -3431,10 +3431,10 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>8.230792776247702</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
@@ -3446,16 +3446,16 @@
         <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>176</v>
+        <v>0.2307927762479889</v>
       </c>
       <c r="O3" t="n">
         <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>28.6</v>
+        <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="R3" t="n">
         <v>0</v>
@@ -3514,13 +3514,13 @@
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>85.38312417100188</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
         <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>23.4</v>
+        <v>0</v>
       </c>
       <c r="N4" t="n">
         <v>0</v>
@@ -3681,25 +3681,25 @@
         <v>48.8</v>
       </c>
       <c r="J2" t="n">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>20.8</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>23.4</v>
+        <v>0</v>
       </c>
       <c r="N2" t="n">
         <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>31.2</v>
+        <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>28.6</v>
+        <v>0</v>
       </c>
       <c r="Q2" t="n">
         <v>0</v>
@@ -3767,7 +3767,7 @@
         <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>23.4</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
         <v>0</v>
@@ -3782,7 +3782,7 @@
         <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="S3" t="n">
         <v>18.4</v>
@@ -3835,10 +3835,10 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
         <v>0</v>
@@ -3853,13 +3853,13 @@
         <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="R4" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="S4" t="n">
         <v>0</v>
@@ -4002,7 +4002,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>95.2</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
@@ -4017,7 +4017,7 @@
         <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>176</v>
+        <v>0</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
@@ -4026,16 +4026,16 @@
         <v>0</v>
       </c>
       <c r="Q2" t="n">
-        <v>118.0342720130611</v>
+        <v>0</v>
       </c>
       <c r="R2" t="n">
         <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>13.2</v>
+        <v>44.23427201306104</v>
       </c>
       <c r="T2" t="n">
-        <v>32</v>
+        <v>20.4</v>
       </c>
       <c r="U2" t="n">
         <v>0</v>
@@ -4109,7 +4109,7 @@
         <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>23.2</v>
+        <v>9.6</v>
       </c>
       <c r="T3" t="n">
         <v>0</v>
@@ -4180,7 +4180,7 @@
         <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="R4" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Reduce number of household types
</commit_message>
<xml_diff>
--- a/model/Output Files/Year 0.xlsx
+++ b/model/Output Files/Year 0.xlsx
@@ -15,12 +15,10 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Feed in from Type 1" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Feed in from Type 2" sheetId="7" state="visible" r:id="rId7"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Feed in from Type 3" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Feed in from Type 4" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Feed in from Type 5" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Costs and Revenues" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Capacities" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Connected Households" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Yearly demand" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Costs and Revenues" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Capacities" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Connected Households" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Yearly demand" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -525,22 +523,22 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>120.0099999999948</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>240</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>120.0099999999948</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>120.0100000000129</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>120.009999999902</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>185.3039999990306</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -564,7 +562,7 @@
         <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>240</v>
       </c>
       <c r="P2" t="n">
         <v>0</v>
@@ -579,22 +577,22 @@
         <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>0</v>
+        <v>240</v>
       </c>
       <c r="U2" t="n">
-        <v>0.7479999996740077</v>
+        <v>0</v>
       </c>
       <c r="V2" t="n">
-        <v>0</v>
+        <v>236.2537743847347</v>
       </c>
       <c r="W2" t="n">
         <v>0</v>
       </c>
       <c r="X2" t="n">
-        <v>0</v>
+        <v>240</v>
       </c>
       <c r="Y2" t="n">
-        <v>0</v>
+        <v>120.0100000000028</v>
       </c>
     </row>
     <row r="3">
@@ -608,7 +606,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>1.102193891711068e-09</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -757,396 +755,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:Y4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="T1" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="U1" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="V1" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="W1" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="X1" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="1" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" t="n">
-        <v>0</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0</v>
-      </c>
-      <c r="V2" t="n">
-        <v>0</v>
-      </c>
-      <c r="W2" t="n">
-        <v>0</v>
-      </c>
-      <c r="X2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R3" t="n">
-        <v>0</v>
-      </c>
-      <c r="S3" t="n">
-        <v>0</v>
-      </c>
-      <c r="T3" t="n">
-        <v>0</v>
-      </c>
-      <c r="U3" t="n">
-        <v>0</v>
-      </c>
-      <c r="V3" t="n">
-        <v>0</v>
-      </c>
-      <c r="W3" t="n">
-        <v>0</v>
-      </c>
-      <c r="X3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R4" t="n">
-        <v>0</v>
-      </c>
-      <c r="S4" t="n">
-        <v>0</v>
-      </c>
-      <c r="T4" t="n">
-        <v>0</v>
-      </c>
-      <c r="U4" t="n">
-        <v>0</v>
-      </c>
-      <c r="V4" t="n">
-        <v>0</v>
-      </c>
-      <c r="W4" t="n">
-        <v>0</v>
-      </c>
-      <c r="X4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Total Revenues</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Total Capital Costs</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Total Operation Variable Costs</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Total Operation Fixed Costs</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Total Profits</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>80569.32880399791</v>
-      </c>
-      <c r="C2" t="n">
-        <v>35800</v>
-      </c>
-      <c r="D2" t="n">
-        <v>15427.52419464854</v>
-      </c>
-      <c r="E2" t="n">
-        <v>9095</v>
-      </c>
-      <c r="F2" t="n">
-        <v>20246.80460934937</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1200,10 +808,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>10163</v>
       </c>
       <c r="C3" t="n">
-        <v>10</v>
+        <v>10173</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -1216,10 +824,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>179</v>
+        <v>5313</v>
       </c>
       <c r="C4" t="n">
-        <v>189</v>
+        <v>5323</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -1230,13 +838,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1296,49 +904,49 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>15</v>
+        <v>840</v>
       </c>
       <c r="C2" t="n">
-        <v>15</v>
+        <v>840</v>
       </c>
       <c r="D2" t="n">
-        <v>15</v>
+        <v>840</v>
       </c>
       <c r="E2" t="n">
-        <v>15</v>
+        <v>840</v>
       </c>
       <c r="F2" t="n">
-        <v>15</v>
+        <v>840</v>
       </c>
       <c r="G2" t="n">
-        <v>15</v>
+        <v>840</v>
       </c>
       <c r="H2" t="n">
-        <v>15</v>
+        <v>840</v>
       </c>
       <c r="I2" t="n">
-        <v>15</v>
+        <v>840</v>
       </c>
       <c r="J2" t="n">
-        <v>15</v>
+        <v>840</v>
       </c>
       <c r="K2" t="n">
-        <v>15</v>
+        <v>840</v>
       </c>
       <c r="L2" t="n">
-        <v>15</v>
+        <v>840</v>
       </c>
       <c r="M2" t="n">
-        <v>15</v>
+        <v>840</v>
       </c>
       <c r="N2" t="n">
-        <v>15</v>
+        <v>840</v>
       </c>
       <c r="O2" t="n">
-        <v>15</v>
+        <v>840</v>
       </c>
       <c r="P2" t="n">
-        <v>15</v>
+        <v>840</v>
       </c>
     </row>
     <row r="3">
@@ -1346,49 +954,49 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>34</v>
+        <v>510</v>
       </c>
       <c r="C3" t="n">
-        <v>34</v>
+        <v>510</v>
       </c>
       <c r="D3" t="n">
-        <v>34</v>
+        <v>510</v>
       </c>
       <c r="E3" t="n">
-        <v>34</v>
+        <v>510</v>
       </c>
       <c r="F3" t="n">
-        <v>34</v>
+        <v>510</v>
       </c>
       <c r="G3" t="n">
-        <v>34</v>
+        <v>484</v>
       </c>
       <c r="H3" t="n">
-        <v>34</v>
+        <v>487</v>
       </c>
       <c r="I3" t="n">
-        <v>34</v>
+        <v>510</v>
       </c>
       <c r="J3" t="n">
-        <v>34</v>
+        <v>510</v>
       </c>
       <c r="K3" t="n">
-        <v>34</v>
+        <v>510</v>
       </c>
       <c r="L3" t="n">
-        <v>34</v>
+        <v>510</v>
       </c>
       <c r="M3" t="n">
-        <v>34</v>
+        <v>510</v>
       </c>
       <c r="N3" t="n">
-        <v>34</v>
+        <v>510</v>
       </c>
       <c r="O3" t="n">
-        <v>34</v>
+        <v>510</v>
       </c>
       <c r="P3" t="n">
-        <v>34</v>
+        <v>510</v>
       </c>
     </row>
     <row r="4">
@@ -1396,149 +1004,49 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="H4" t="n">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="J4" t="n">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="K4" t="n">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="L4" t="n">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="M4" t="n">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="N4" t="n">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="O4" t="n">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="P4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>4</v>
-      </c>
-      <c r="C5" t="n">
-        <v>4</v>
-      </c>
-      <c r="D5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F5" t="n">
-        <v>4</v>
-      </c>
-      <c r="G5" t="n">
-        <v>4</v>
-      </c>
-      <c r="H5" t="n">
-        <v>4</v>
-      </c>
-      <c r="I5" t="n">
-        <v>4</v>
-      </c>
-      <c r="J5" t="n">
-        <v>4</v>
-      </c>
-      <c r="K5" t="n">
-        <v>4</v>
-      </c>
-      <c r="L5" t="n">
-        <v>4</v>
-      </c>
-      <c r="M5" t="n">
-        <v>4</v>
-      </c>
-      <c r="N5" t="n">
-        <v>4</v>
-      </c>
-      <c r="O5" t="n">
-        <v>4</v>
-      </c>
-      <c r="P5" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>11</v>
-      </c>
-      <c r="C6" t="n">
-        <v>11</v>
-      </c>
-      <c r="D6" t="n">
-        <v>11</v>
-      </c>
-      <c r="E6" t="n">
-        <v>11</v>
-      </c>
-      <c r="F6" t="n">
-        <v>11</v>
-      </c>
-      <c r="G6" t="n">
-        <v>11</v>
-      </c>
-      <c r="H6" t="n">
-        <v>11</v>
-      </c>
-      <c r="I6" t="n">
-        <v>11</v>
-      </c>
-      <c r="J6" t="n">
-        <v>11</v>
-      </c>
-      <c r="K6" t="n">
-        <v>11</v>
-      </c>
-      <c r="L6" t="n">
-        <v>11</v>
-      </c>
-      <c r="M6" t="n">
-        <v>11</v>
-      </c>
-      <c r="N6" t="n">
-        <v>11</v>
-      </c>
-      <c r="O6" t="n">
-        <v>11</v>
-      </c>
-      <c r="P6" t="n">
-        <v>11</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1546,7 +1054,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1639,76 +1147,76 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>-32.5</v>
+        <v>-1211.51</v>
       </c>
       <c r="C2" t="n">
-        <v>-19.5</v>
+        <v>-1136.26</v>
       </c>
       <c r="D2" t="n">
-        <v>-13</v>
+        <v>-1061.81</v>
       </c>
       <c r="E2" t="n">
-        <v>-13</v>
+        <v>-996.17</v>
       </c>
       <c r="F2" t="n">
-        <v>-13</v>
+        <v>-977.63</v>
       </c>
       <c r="G2" t="n">
-        <v>22.1</v>
+        <v>-866.895</v>
       </c>
       <c r="H2" t="n">
-        <v>50.7</v>
+        <v>-775.78</v>
       </c>
       <c r="I2" t="n">
-        <v>26</v>
+        <v>-566.6700000000001</v>
       </c>
       <c r="J2" t="n">
-        <v>27.3</v>
+        <v>-390.5800000000002</v>
       </c>
       <c r="K2" t="n">
-        <v>80.59999999999999</v>
+        <v>-468.3050000000001</v>
       </c>
       <c r="L2" t="n">
-        <v>114.4</v>
+        <v>-559.8699999999999</v>
       </c>
       <c r="M2" t="n">
-        <v>128.7</v>
+        <v>-699.625</v>
       </c>
       <c r="N2" t="n">
-        <v>143</v>
+        <v>-920.71</v>
       </c>
       <c r="O2" t="n">
-        <v>109.2</v>
+        <v>-1118.445</v>
       </c>
       <c r="P2" t="n">
-        <v>94.90000000000001</v>
+        <v>-1160.89</v>
       </c>
       <c r="Q2" t="n">
-        <v>80.59999999999999</v>
+        <v>-1156.31</v>
       </c>
       <c r="R2" t="n">
-        <v>19.5</v>
+        <v>-1141.46</v>
       </c>
       <c r="S2" t="n">
-        <v>-41.60000000000001</v>
+        <v>-1144.01</v>
       </c>
       <c r="T2" t="n">
-        <v>-88.40000000000001</v>
+        <v>-1289.76</v>
       </c>
       <c r="U2" t="n">
-        <v>-117</v>
+        <v>-1379.2</v>
       </c>
       <c r="V2" t="n">
-        <v>-97.5</v>
+        <v>-1346.75</v>
       </c>
       <c r="W2" t="n">
-        <v>-78</v>
+        <v>-1297.99</v>
       </c>
       <c r="X2" t="n">
-        <v>-52</v>
+        <v>-1140.13</v>
       </c>
       <c r="Y2" t="n">
-        <v>-39</v>
+        <v>-1064.46</v>
       </c>
     </row>
     <row r="3">
@@ -1716,76 +1224,76 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-32.5</v>
+        <v>-879.3</v>
       </c>
       <c r="C3" t="n">
-        <v>-19.5</v>
+        <v>-811</v>
       </c>
       <c r="D3" t="n">
-        <v>-13</v>
+        <v>-743.5</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>-620.6500000000001</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>-335.1400000000001</v>
       </c>
       <c r="G3" t="n">
-        <v>-19.5</v>
+        <v>27.27000000000005</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>193.87</v>
       </c>
       <c r="I3" t="n">
-        <v>83.2</v>
+        <v>379.3449999999998</v>
       </c>
       <c r="J3" t="n">
-        <v>124.8</v>
+        <v>534.7799999999999</v>
       </c>
       <c r="K3" t="n">
-        <v>166.4</v>
+        <v>483.6749999999999</v>
       </c>
       <c r="L3" t="n">
-        <v>187.2</v>
+        <v>452.2999999999998</v>
       </c>
       <c r="M3" t="n">
-        <v>149.5</v>
+        <v>367.57</v>
       </c>
       <c r="N3" t="n">
-        <v>101.4</v>
+        <v>149.0700000000001</v>
       </c>
       <c r="O3" t="n">
-        <v>145.6</v>
+        <v>-161.885</v>
       </c>
       <c r="P3" t="n">
-        <v>32.49999999999999</v>
+        <v>-461.76</v>
       </c>
       <c r="Q3" t="n">
-        <v>39</v>
+        <v>-820.285</v>
       </c>
       <c r="R3" t="n">
-        <v>62.4</v>
+        <v>-932.5600000000001</v>
       </c>
       <c r="S3" t="n">
-        <v>-62.40000000000001</v>
+        <v>-950.8</v>
       </c>
       <c r="T3" t="n">
-        <v>-130</v>
+        <v>-1103.5</v>
       </c>
       <c r="U3" t="n">
-        <v>0</v>
+        <v>-1198.5</v>
       </c>
       <c r="V3" t="n">
-        <v>0</v>
+        <v>-1173</v>
       </c>
       <c r="W3" t="n">
-        <v>-78</v>
+        <v>-1129.8</v>
       </c>
       <c r="X3" t="n">
-        <v>0</v>
+        <v>-977.5</v>
       </c>
       <c r="Y3" t="n">
-        <v>-39</v>
+        <v>-906</v>
       </c>
     </row>
     <row r="4">
@@ -1793,76 +1301,76 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-32.5</v>
+        <v>-1150.35</v>
       </c>
       <c r="C4" t="n">
-        <v>-19.5</v>
+        <v>-1086.22</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>-1021.5</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>-966.9799999999999</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>-861.235</v>
       </c>
       <c r="G4" t="n">
-        <v>-19.5</v>
+        <v>-428.7049999999999</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>-144.71</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>96.98000000000013</v>
       </c>
       <c r="J4" t="n">
-        <v>20.8</v>
+        <v>278.04</v>
       </c>
       <c r="K4" t="n">
-        <v>83.2</v>
+        <v>230.71</v>
       </c>
       <c r="L4" t="n">
-        <v>145.6</v>
+        <v>187.8149999999999</v>
       </c>
       <c r="M4" t="n">
-        <v>107.9</v>
+        <v>79.84499999999994</v>
       </c>
       <c r="N4" t="n">
-        <v>166.4</v>
+        <v>-180.765</v>
       </c>
       <c r="O4" t="n">
-        <v>145.6</v>
+        <v>-573.1600000000001</v>
       </c>
       <c r="P4" t="n">
-        <v>83.2</v>
+        <v>-991.62</v>
       </c>
       <c r="Q4" t="n">
-        <v>41.6</v>
+        <v>-1263.34</v>
       </c>
       <c r="R4" t="n">
-        <v>20.8</v>
+        <v>-1258.22</v>
       </c>
       <c r="S4" t="n">
-        <v>0</v>
+        <v>-1269.11</v>
       </c>
       <c r="T4" t="n">
-        <v>-130</v>
+        <v>-1424.59</v>
       </c>
       <c r="U4" t="n">
-        <v>0</v>
+        <v>-1520.98</v>
       </c>
       <c r="V4" t="n">
-        <v>0</v>
+        <v>-1498.26</v>
       </c>
       <c r="W4" t="n">
-        <v>0</v>
+        <v>-1456.45</v>
       </c>
       <c r="X4" t="n">
-        <v>0</v>
+        <v>-1306.93</v>
       </c>
       <c r="Y4" t="n">
-        <v>-39</v>
+        <v>-1236.82</v>
       </c>
     </row>
   </sheetData>
@@ -1978,46 +1486,46 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>2</v>
+        <v>681.5910000000275</v>
       </c>
       <c r="H2" t="n">
-        <v>4</v>
+        <v>1912.524000000063</v>
       </c>
       <c r="I2" t="n">
-        <v>5</v>
+        <v>3153.630000000094</v>
       </c>
       <c r="J2" t="n">
-        <v>6</v>
+        <v>3926.778000000103</v>
       </c>
       <c r="K2" t="n">
-        <v>7</v>
+        <v>4038.68100000009</v>
       </c>
       <c r="L2" t="n">
-        <v>8</v>
+        <v>3560.55</v>
       </c>
       <c r="M2" t="n">
-        <v>8.999999999999996</v>
+        <v>2675.499000000122</v>
       </c>
       <c r="N2" t="n">
-        <v>10</v>
+        <v>1607.334000000046</v>
       </c>
       <c r="O2" t="n">
-        <v>8.999999999999996</v>
+        <v>640.8990000000266</v>
       </c>
       <c r="P2" t="n">
-        <v>8</v>
+        <v>20.3460000000009</v>
       </c>
       <c r="Q2" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U2" t="n">
         <v>0</v>
@@ -2049,49 +1557,49 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>305.1900000000139</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>1586.988000000005</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>504</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>630</v>
       </c>
       <c r="I3" t="n">
-        <v>4</v>
+        <v>5969.8</v>
       </c>
       <c r="J3" t="n">
-        <v>6</v>
+        <v>2801.011999999985</v>
       </c>
       <c r="K3" t="n">
-        <v>8</v>
+        <v>798</v>
       </c>
       <c r="L3" t="n">
-        <v>9</v>
+        <v>3750.747984894617</v>
       </c>
       <c r="M3" t="n">
-        <v>9.999999999999996</v>
+        <v>756</v>
       </c>
       <c r="N3" t="n">
-        <v>8</v>
+        <v>756</v>
       </c>
       <c r="O3" t="n">
-        <v>7</v>
+        <v>739.2</v>
       </c>
       <c r="P3" t="n">
-        <v>5</v>
+        <v>672</v>
       </c>
       <c r="Q3" t="n">
-        <v>5</v>
+        <v>600.2070000000257</v>
       </c>
       <c r="R3" t="n">
-        <v>3</v>
+        <v>40.69200000000179</v>
       </c>
       <c r="S3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T3" t="n">
         <v>0</v>
@@ -2129,43 +1637,43 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>457.7849999994903</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>677.8799999996648</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>805.5600000007973</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>6147.040000000002</v>
       </c>
       <c r="J4" t="n">
-        <v>1</v>
+        <v>2706.256266196849</v>
       </c>
       <c r="K4" t="n">
-        <v>4</v>
+        <v>978.6</v>
       </c>
       <c r="L4" t="n">
-        <v>7</v>
+        <v>6303.280000000002</v>
       </c>
       <c r="M4" t="n">
-        <v>8</v>
+        <v>5643.37500000048</v>
       </c>
       <c r="N4" t="n">
-        <v>8</v>
+        <v>940.8</v>
       </c>
       <c r="O4" t="n">
-        <v>7</v>
+        <v>925.6800000000574</v>
       </c>
       <c r="P4" t="n">
-        <v>4</v>
+        <v>1018.259999999893</v>
       </c>
       <c r="Q4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4" t="n">
         <v>0</v>
@@ -2290,7 +1798,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>-5.384208634495735e-08</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -2305,31 +1813,31 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>1136.744000000566</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>2586.960000003307</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>3536.198000000803</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>3570.375999999332</v>
       </c>
       <c r="L2" t="n">
-        <v>122.4000000001863</v>
+        <v>3000.680000001536</v>
       </c>
       <c r="M2" t="n">
-        <v>137.7</v>
+        <v>1975.874000003975</v>
       </c>
       <c r="N2" t="n">
-        <v>153</v>
+        <v>686.6240000014985</v>
       </c>
       <c r="O2" t="n">
-        <v>118.2000000002561</v>
+        <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>79.60909090864855</v>
+        <v>0</v>
       </c>
       <c r="Q2" t="n">
         <v>0</v>
@@ -2353,7 +1861,7 @@
         <v>0</v>
       </c>
       <c r="X2" t="n">
-        <v>0</v>
+        <v>2.328306436538696e-09</v>
       </c>
       <c r="Y2" t="n">
         <v>0</v>
@@ -2376,7 +1884,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>1124.988000000005</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -2385,34 +1893,34 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>4</v>
+        <v>5323</v>
       </c>
       <c r="J3" t="n">
-        <v>6</v>
+        <v>2129.011999999985</v>
       </c>
       <c r="K3" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>174.8571574291427</v>
+        <v>2952.747984894617</v>
       </c>
       <c r="M3" t="n">
-        <v>159.5000000037486</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
         <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>37.49999999999999</v>
+        <v>0</v>
       </c>
       <c r="Q3" t="n">
         <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S3" t="n">
         <v>0</v>
@@ -2462,34 +1970,34 @@
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>5323</v>
       </c>
       <c r="J4" t="n">
-        <v>1</v>
+        <v>1855.336266196784</v>
       </c>
       <c r="K4" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>7</v>
+        <v>5323</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>4704.25500000048</v>
       </c>
       <c r="N4" t="n">
-        <v>174.4000000002561</v>
+        <v>0</v>
       </c>
       <c r="O4" t="n">
-        <v>50.98312417081809</v>
+        <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R4" t="n">
-        <v>2.000000000000057</v>
+        <v>0</v>
       </c>
       <c r="S4" t="n">
         <v>0</v>
@@ -2611,19 +2119,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>32.5</v>
+        <v>1091.5</v>
       </c>
       <c r="C2" t="n">
-        <v>19.50000000004657</v>
+        <v>896.2599999486321</v>
       </c>
       <c r="D2" t="n">
-        <v>12.99999999995343</v>
+        <v>941.8</v>
       </c>
       <c r="E2" t="n">
-        <v>12.99999999995343</v>
+        <v>876.1599999999908</v>
       </c>
       <c r="F2" t="n">
-        <v>12.99999999995343</v>
+        <v>857.6200000002173</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -2650,37 +2158,37 @@
         <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>237.5459999969</v>
       </c>
       <c r="P2" t="n">
-        <v>0</v>
+        <v>1140.543999999999</v>
       </c>
       <c r="Q2" t="n">
-        <v>0</v>
+        <v>1156.31000000014</v>
       </c>
       <c r="R2" t="n">
-        <v>0</v>
+        <v>1141.460000000001</v>
       </c>
       <c r="S2" t="n">
-        <v>38.59999999974389</v>
+        <v>1144.01</v>
       </c>
       <c r="T2" t="n">
-        <v>86.40000000000001</v>
+        <v>1049.76</v>
       </c>
       <c r="U2" t="n">
-        <v>116.2520000003726</v>
+        <v>1379.2</v>
       </c>
       <c r="V2" t="n">
-        <v>97.5</v>
+        <v>1110.496225615265</v>
       </c>
       <c r="W2" t="n">
-        <v>77.99999999995343</v>
+        <v>1297.99</v>
       </c>
       <c r="X2" t="n">
-        <v>52.00000000004657</v>
+        <v>900.1300000023284</v>
       </c>
       <c r="Y2" t="n">
-        <v>38.99999999997672</v>
+        <v>944.45</v>
       </c>
     </row>
     <row r="3">
@@ -2688,22 +2196,22 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>32.5</v>
+        <v>879.3</v>
       </c>
       <c r="C3" t="n">
-        <v>19.50000000004657</v>
+        <v>811.000000001378</v>
       </c>
       <c r="D3" t="n">
-        <v>12.99999999995343</v>
+        <v>743.4999999988978</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>315.4599999966101</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>19.50000000004657</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -2733,31 +2241,31 @@
         <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>0</v>
+        <v>220.0779999986006</v>
       </c>
       <c r="R3" t="n">
-        <v>0</v>
+        <v>891.8679999999982</v>
       </c>
       <c r="S3" t="n">
-        <v>60.4</v>
+        <v>950.8</v>
       </c>
       <c r="T3" t="n">
-        <v>130</v>
+        <v>1103.5</v>
       </c>
       <c r="U3" t="n">
-        <v>0</v>
+        <v>1198.5</v>
       </c>
       <c r="V3" t="n">
-        <v>0</v>
+        <v>1173</v>
       </c>
       <c r="W3" t="n">
-        <v>77.99999999995343</v>
+        <v>1129.8</v>
       </c>
       <c r="X3" t="n">
-        <v>0</v>
+        <v>977.5</v>
       </c>
       <c r="Y3" t="n">
-        <v>38.99999999997672</v>
+        <v>906</v>
       </c>
     </row>
     <row r="4">
@@ -2765,22 +2273,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>32.5</v>
+        <v>1150.35</v>
       </c>
       <c r="C4" t="n">
-        <v>19.50000000004657</v>
+        <v>1086.22</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1021.5</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>966.9799999999973</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>403.45</v>
       </c>
       <c r="G4" t="n">
-        <v>19.50000000004657</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -2810,31 +2318,31 @@
         <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>0</v>
+        <v>1263.34</v>
       </c>
       <c r="R4" t="n">
-        <v>0</v>
+        <v>1258.22</v>
       </c>
       <c r="S4" t="n">
-        <v>0</v>
+        <v>1269.11</v>
       </c>
       <c r="T4" t="n">
-        <v>130</v>
+        <v>1424.59</v>
       </c>
       <c r="U4" t="n">
-        <v>0</v>
+        <v>1520.98</v>
       </c>
       <c r="V4" t="n">
-        <v>0</v>
+        <v>1498.26</v>
       </c>
       <c r="W4" t="n">
-        <v>0</v>
+        <v>1456.45</v>
       </c>
       <c r="X4" t="n">
-        <v>0</v>
+        <v>1306.929999999997</v>
       </c>
       <c r="Y4" t="n">
-        <v>38.99999999997672</v>
+        <v>1236.82</v>
       </c>
     </row>
   </sheetData>
@@ -2935,76 +2443,76 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>210.290909090815</v>
+        <v>7866.319191918572</v>
       </c>
       <c r="C2" t="n">
-        <v>190.5939393937983</v>
+        <v>6961.006060606524</v>
       </c>
       <c r="D2" t="n">
-        <v>177.4626262625322</v>
+        <v>6009.692929293387</v>
       </c>
       <c r="E2" t="n">
-        <v>164.3313131312661</v>
+        <v>5124.682828283299</v>
       </c>
       <c r="F2" t="n">
-        <v>151.2</v>
+        <v>4258.4</v>
       </c>
       <c r="G2" t="n">
-        <v>151.2</v>
+        <v>4258.4</v>
       </c>
       <c r="H2" t="n">
-        <v>151.2</v>
+        <v>5383.776560000812</v>
       </c>
       <c r="I2" t="n">
-        <v>151.2</v>
+        <v>7944.866960004087</v>
       </c>
       <c r="J2" t="n">
-        <v>151.2</v>
+        <v>11445.70298000488</v>
       </c>
       <c r="K2" t="n">
-        <v>151.2</v>
+        <v>14980.37522000566</v>
       </c>
       <c r="L2" t="n">
-        <v>272.3760000001844</v>
+        <v>17951.04842000718</v>
       </c>
       <c r="M2" t="n">
-        <v>408.6990000001844</v>
+        <v>19907.16368001112</v>
       </c>
       <c r="N2" t="n">
-        <v>560.1690000001844</v>
+        <v>20586.9214400126</v>
       </c>
       <c r="O2" t="n">
-        <v>677.1870000004379</v>
+        <v>20346.97598547028</v>
       </c>
       <c r="P2" t="n">
-        <v>756</v>
+        <v>19194.91133900563</v>
       </c>
       <c r="Q2" t="n">
-        <v>756</v>
+        <v>18026.92144001559</v>
       </c>
       <c r="R2" t="n">
-        <v>756</v>
+        <v>16873.93154102569</v>
       </c>
       <c r="S2" t="n">
-        <v>717.0101010103597</v>
+        <v>15718.36588446004</v>
       </c>
       <c r="T2" t="n">
-        <v>629.7373737376324</v>
+        <v>14658.0022480964</v>
       </c>
       <c r="U2" t="n">
-        <v>512.3111111109935</v>
+        <v>13264.87093496496</v>
       </c>
       <c r="V2" t="n">
-        <v>413.826262626145</v>
+        <v>12143.15757575762</v>
       </c>
       <c r="W2" t="n">
-        <v>335.0383838383133</v>
+        <v>10832.05656565661</v>
       </c>
       <c r="X2" t="n">
-        <v>282.5131313130137</v>
+        <v>9922.834343434341</v>
       </c>
       <c r="Y2" t="n">
-        <v>243.1191919190979</v>
+        <v>8968.844444444445</v>
       </c>
     </row>
     <row r="3">
@@ -3012,76 +2520,76 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>203.7252525252996</v>
+        <v>6147.248484845339</v>
       </c>
       <c r="C3" t="n">
-        <v>184.0282828282828</v>
+        <v>5328.056565652028</v>
       </c>
       <c r="D3" t="n">
-        <v>170.8969696970167</v>
+        <v>4577.04646464304</v>
       </c>
       <c r="E3" t="n">
-        <v>170.8969696970167</v>
+        <v>4258.4</v>
       </c>
       <c r="F3" t="n">
-        <v>170.8969696970167</v>
+        <v>5372.138120000014</v>
       </c>
       <c r="G3" t="n">
-        <v>151.2</v>
+        <v>5372.138120000014</v>
       </c>
       <c r="H3" t="n">
-        <v>151.2</v>
+        <v>5372.138120000117</v>
       </c>
       <c r="I3" t="n">
-        <v>155.16</v>
+        <v>10641.90812000001</v>
       </c>
       <c r="J3" t="n">
-        <v>161.1</v>
+        <v>12749.63</v>
       </c>
       <c r="K3" t="n">
-        <v>169.02</v>
+        <v>12749.63</v>
       </c>
       <c r="L3" t="n">
-        <v>342.1285858548513</v>
+        <v>15672.85050504567</v>
       </c>
       <c r="M3" t="n">
-        <v>500.0335858585624</v>
+        <v>15672.85050504567</v>
       </c>
       <c r="N3" t="n">
-        <v>500.0335858585624</v>
+        <v>15672.85050504567</v>
       </c>
       <c r="O3" t="n">
-        <v>506.9635858585624</v>
+        <v>15672.85050504567</v>
       </c>
       <c r="P3" t="n">
-        <v>544.0885858585624</v>
+        <v>15672.85050504567</v>
       </c>
       <c r="Q3" t="n">
-        <v>544.0885858585624</v>
+        <v>15450.54949494608</v>
       </c>
       <c r="R3" t="n">
-        <v>547.0585858585624</v>
+        <v>14549.67272726931</v>
       </c>
       <c r="S3" t="n">
-        <v>486.0484848484614</v>
+        <v>13589.26868686528</v>
       </c>
       <c r="T3" t="n">
-        <v>354.73535353533</v>
+        <v>12474.62222221882</v>
       </c>
       <c r="U3" t="n">
-        <v>354.73535353533</v>
+        <v>11264.01616161301</v>
       </c>
       <c r="V3" t="n">
-        <v>354.73535353533</v>
+        <v>10079.16767676453</v>
       </c>
       <c r="W3" t="n">
-        <v>275.9474747474983</v>
+        <v>8937.955555552406</v>
       </c>
       <c r="X3" t="n">
-        <v>275.9474747474983</v>
+        <v>7950.58181817867</v>
       </c>
       <c r="Y3" t="n">
-        <v>236.5535353535824</v>
+        <v>7035.430303027157</v>
       </c>
     </row>
     <row r="4">
@@ -3089,76 +2597,76 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>190.5939393940335</v>
+        <v>7771.682828282733</v>
       </c>
       <c r="C4" t="n">
-        <v>170.8969696970167</v>
+        <v>6674.490909090813</v>
       </c>
       <c r="D4" t="n">
-        <v>170.8969696970167</v>
+        <v>5642.67272727324</v>
       </c>
       <c r="E4" t="n">
-        <v>170.8969696970167</v>
+        <v>4665.925252525767</v>
       </c>
       <c r="F4" t="n">
-        <v>170.8969696970167</v>
+        <v>4258.4</v>
       </c>
       <c r="G4" t="n">
-        <v>151.2</v>
+        <v>4258.4</v>
       </c>
       <c r="H4" t="n">
-        <v>151.2</v>
+        <v>4258.4</v>
       </c>
       <c r="I4" t="n">
-        <v>151.2</v>
+        <v>9528.17000000046</v>
       </c>
       <c r="J4" t="n">
-        <v>152.19</v>
+        <v>11364.95290353488</v>
       </c>
       <c r="K4" t="n">
-        <v>156.15</v>
+        <v>11364.95290353488</v>
       </c>
       <c r="L4" t="n">
-        <v>163.08</v>
+        <v>16634.72290353488</v>
       </c>
       <c r="M4" t="n">
-        <v>163.08</v>
+        <v>21291.93535353536</v>
       </c>
       <c r="N4" t="n">
-        <v>335.7360000002536</v>
+        <v>21291.93535353536</v>
       </c>
       <c r="O4" t="n">
-        <v>386.2092929293635</v>
+        <v>21291.93535353536</v>
       </c>
       <c r="P4" t="n">
-        <v>390.1692929293635</v>
+        <v>21291.93535353525</v>
       </c>
       <c r="Q4" t="n">
-        <v>392.1492929293635</v>
+        <v>20015.83434343424</v>
       </c>
       <c r="R4" t="n">
-        <v>394.1292929293635</v>
+        <v>18744.90505050495</v>
       </c>
       <c r="S4" t="n">
-        <v>394.1292929293635</v>
+        <v>17462.97575757566</v>
       </c>
       <c r="T4" t="n">
-        <v>262.8161616162322</v>
+        <v>16023.99595959586</v>
       </c>
       <c r="U4" t="n">
-        <v>262.8161616162322</v>
+        <v>14487.65252525243</v>
       </c>
       <c r="V4" t="n">
-        <v>262.8161616162322</v>
+        <v>12974.25858585849</v>
       </c>
       <c r="W4" t="n">
-        <v>262.8161616162322</v>
+        <v>11503.09696969687</v>
       </c>
       <c r="X4" t="n">
-        <v>262.8161616162322</v>
+        <v>10182.96565656556</v>
       </c>
       <c r="Y4" t="n">
-        <v>223.4222222223163</v>
+        <v>8933.65252525243</v>
       </c>
     </row>
     <row r="5">
@@ -6838,34 +6346,34 @@
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>26.2</v>
+        <v>146.3700000011595</v>
       </c>
       <c r="J2" t="n">
-        <v>33</v>
+        <v>311.1</v>
       </c>
       <c r="K2" t="n">
-        <v>19</v>
+        <v>349.0950000006674</v>
       </c>
       <c r="L2" t="n">
-        <v>108.8000000002794</v>
+        <v>268.7700000011828</v>
       </c>
       <c r="M2" t="n">
-        <v>122.3999999995809</v>
+        <v>116.5350000018088</v>
       </c>
       <c r="N2" t="n">
-        <v>136</v>
+        <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>112.2000000001863</v>
+        <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>98.60000000020955</v>
+        <v>0</v>
       </c>
       <c r="Q2" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>28.8</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
         <v>0</v>
@@ -6924,22 +6432,22 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>153</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>139.4000000037486</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="O3" t="n">
         <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>47.60000000020955</v>
+        <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="R3" t="n">
         <v>0</v>
@@ -7004,13 +6512,13 @@
         <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>15.4</v>
+        <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>136</v>
+        <v>0</v>
       </c>
       <c r="O4" t="n">
-        <v>43.98312417081809</v>
+        <v>0</v>
       </c>
       <c r="P4" t="n">
         <v>0</v>
@@ -7019,7 +6527,7 @@
         <v>0</v>
       </c>
       <c r="R4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4" t="n">
         <v>0</v>
@@ -7156,34 +6664,34 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>1.700000000186265</v>
+        <v>6.360000001499429</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>49.04000000050291</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>100.0800000020536</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>130.7600000002421</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>136</v>
       </c>
       <c r="L2" t="n">
-        <v>7.200000000186265</v>
+        <v>118.8800000002375</v>
       </c>
       <c r="M2" t="n">
-        <v>8.100000000209548</v>
+        <v>84.32000000204425</v>
       </c>
       <c r="N2" t="n">
-        <v>9</v>
+        <v>42.56000000145286</v>
       </c>
       <c r="O2" t="n">
-        <v>7.800000000279397</v>
+        <v>4.800000003073364</v>
       </c>
       <c r="P2" t="n">
-        <v>1.609090908439015</v>
+        <v>0</v>
       </c>
       <c r="Q2" t="n">
         <v>0</v>
@@ -7192,7 +6700,7 @@
         <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>1.400000000256114</v>
+        <v>0</v>
       </c>
       <c r="T2" t="n">
         <v>0</v>
@@ -7227,7 +6735,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>2.00000000337088</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -7251,7 +6759,7 @@
         <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>9.099999999743886</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
         <v>0</v>
@@ -7260,16 +6768,16 @@
         <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>3.900000000256114</v>
+        <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>0</v>
+        <v>11.6000000013737</v>
       </c>
       <c r="R3" t="n">
         <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>0.3999999999999999</v>
+        <v>0</v>
       </c>
       <c r="T3" t="n">
         <v>0</v>
@@ -7331,7 +6839,7 @@
         <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="O4" t="n">
         <v>0</v>
@@ -7378,7 +6886,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7387,77 +6895,30 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="T1" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="U1" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="V1" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="W1" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="X1" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="1" t="n">
-        <v>23</v>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Total Revenues</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Total Capital Costs</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Total Operation Variable Costs</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Total Operation Fixed Costs</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Total Profits</t>
+        </is>
       </c>
     </row>
     <row r="2">
@@ -7465,230 +6926,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>3375173.553962285</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>4111500</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>427018.4369220809</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>187210</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>4.099999999813735</v>
-      </c>
-      <c r="H2" t="n">
-        <v>9</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" t="n">
-        <v>19.1999999997206</v>
-      </c>
-      <c r="M2" t="n">
-        <v>21.60000000020955</v>
-      </c>
-      <c r="N2" t="n">
-        <v>24</v>
-      </c>
-      <c r="O2" t="n">
-        <v>20.39999999979045</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2" t="n">
-        <v>2</v>
-      </c>
-      <c r="T2" t="n">
-        <v>0</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0</v>
-      </c>
-      <c r="V2" t="n">
-        <v>0</v>
-      </c>
-      <c r="W2" t="n">
-        <v>0</v>
-      </c>
-      <c r="X2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" t="n">
-        <v>12.85715742914272</v>
-      </c>
-      <c r="M3" t="n">
-        <v>24.40000000025611</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" t="n">
-        <v>9.599999999534333</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R3" t="n">
-        <v>0</v>
-      </c>
-      <c r="S3" t="n">
-        <v>0</v>
-      </c>
-      <c r="T3" t="n">
-        <v>0</v>
-      </c>
-      <c r="U3" t="n">
-        <v>0</v>
-      </c>
-      <c r="V3" t="n">
-        <v>0</v>
-      </c>
-      <c r="W3" t="n">
-        <v>0</v>
-      </c>
-      <c r="X3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" t="n">
-        <v>22.40000000025611</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>0</v>
-      </c>
-      <c r="R4" t="n">
-        <v>0</v>
-      </c>
-      <c r="S4" t="n">
-        <v>0</v>
-      </c>
-      <c r="T4" t="n">
-        <v>0</v>
-      </c>
-      <c r="U4" t="n">
-        <v>0</v>
-      </c>
-      <c r="V4" t="n">
-        <v>0</v>
-      </c>
-      <c r="W4" t="n">
-        <v>0</v>
-      </c>
-      <c r="X4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>0</v>
+        <v>-1350554.882959796</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
increase number of household types
</commit_message>
<xml_diff>
--- a/model/Output Files/Year 0.xlsx
+++ b/model/Output Files/Year 0.xlsx
@@ -15,10 +15,11 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Feed in from Type 1" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Feed in from Type 2" sheetId="7" state="visible" r:id="rId7"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Feed in from Type 3" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Costs and Revenues" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Capacities" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Connected Households" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Yearly demand" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Feed in from Type 4" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Costs and Revenues" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Capacities" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Connected Households" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Yearly demand" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -523,52 +524,52 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>120.0100000000238</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>240</v>
+      </c>
+      <c r="G2" t="n">
+        <v>120.0099999996673</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>160.8283227917981</v>
+      </c>
+      <c r="P2" t="n">
+        <v>240</v>
+      </c>
+      <c r="Q2" t="n">
         <v>120.0099999999948</v>
-      </c>
-      <c r="C2" t="n">
-        <v>240</v>
-      </c>
-      <c r="D2" t="n">
-        <v>120.0099999999948</v>
-      </c>
-      <c r="E2" t="n">
-        <v>120.0100000000129</v>
-      </c>
-      <c r="F2" t="n">
-        <v>120.009999999902</v>
-      </c>
-      <c r="G2" t="n">
-        <v>185.3039999990306</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" t="n">
-        <v>240</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>0</v>
       </c>
       <c r="R2" t="n">
         <v>0</v>
@@ -580,19 +581,19 @@
         <v>240</v>
       </c>
       <c r="U2" t="n">
-        <v>0</v>
+        <v>240</v>
       </c>
       <c r="V2" t="n">
-        <v>236.2537743847347</v>
+        <v>0</v>
       </c>
       <c r="W2" t="n">
-        <v>0</v>
+        <v>240</v>
       </c>
       <c r="X2" t="n">
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="Y2" t="n">
-        <v>120.0100000000028</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -606,7 +607,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>1.102193891711068e-09</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -737,7 +738,7 @@
         <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>0</v>
+        <v>3.960000000061656</v>
       </c>
       <c r="W4" t="n">
         <v>0</v>
@@ -746,7 +747,7 @@
         <v>0</v>
       </c>
       <c r="Y4" t="n">
-        <v>0</v>
+        <v>135.5230000000026</v>
       </c>
     </row>
   </sheetData>
@@ -755,6 +756,72 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Total Revenues</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Total Capital Costs</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Total Operation Variable Costs</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Total Operation Fixed Costs</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Total Profits</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>3384768.432639945</v>
+      </c>
+      <c r="C2" t="n">
+        <v>4116600</v>
+      </c>
+      <c r="D2" t="n">
+        <v>426727.3103897487</v>
+      </c>
+      <c r="E2" t="n">
+        <v>187585</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-1346143.877749803</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -808,10 +875,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10163</v>
+        <v>10196</v>
       </c>
       <c r="C3" t="n">
-        <v>10173</v>
+        <v>10206</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -824,10 +891,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5313</v>
+        <v>5289</v>
       </c>
       <c r="C4" t="n">
-        <v>5323</v>
+        <v>5299</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -838,13 +905,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -969,16 +1036,16 @@
         <v>510</v>
       </c>
       <c r="G3" t="n">
-        <v>484</v>
+        <v>510</v>
       </c>
       <c r="H3" t="n">
-        <v>487</v>
+        <v>510</v>
       </c>
       <c r="I3" t="n">
         <v>510</v>
       </c>
       <c r="J3" t="n">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="K3" t="n">
         <v>510</v>
@@ -1019,16 +1086,16 @@
         <v>40</v>
       </c>
       <c r="G4" t="n">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="H4" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I4" t="n">
         <v>40</v>
       </c>
       <c r="J4" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="K4" t="n">
         <v>40</v>
@@ -1047,6 +1114,56 @@
       </c>
       <c r="P4" t="n">
         <v>40</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" t="n">
+        <v>1</v>
+      </c>
+      <c r="P5" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1054,7 +1171,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1156,43 +1273,43 @@
         <v>-1061.81</v>
       </c>
       <c r="E2" t="n">
-        <v>-996.17</v>
+        <v>-1031.17</v>
       </c>
       <c r="F2" t="n">
         <v>-977.63</v>
       </c>
       <c r="G2" t="n">
-        <v>-866.895</v>
+        <v>-858.895</v>
       </c>
       <c r="H2" t="n">
-        <v>-775.78</v>
+        <v>-752.78</v>
       </c>
       <c r="I2" t="n">
-        <v>-566.6700000000001</v>
+        <v>-528.6700000000001</v>
       </c>
       <c r="J2" t="n">
-        <v>-390.5800000000002</v>
+        <v>-343.5800000000002</v>
       </c>
       <c r="K2" t="n">
-        <v>-468.3050000000001</v>
+        <v>-420.3050000000001</v>
       </c>
       <c r="L2" t="n">
-        <v>-559.8699999999999</v>
+        <v>-516.8699999999999</v>
       </c>
       <c r="M2" t="n">
-        <v>-699.625</v>
+        <v>-667.625</v>
       </c>
       <c r="N2" t="n">
-        <v>-920.71</v>
+        <v>-901.71</v>
       </c>
       <c r="O2" t="n">
-        <v>-1118.445</v>
+        <v>-1111.445</v>
       </c>
       <c r="P2" t="n">
         <v>-1160.89</v>
       </c>
       <c r="Q2" t="n">
-        <v>-1156.31</v>
+        <v>-1191.31</v>
       </c>
       <c r="R2" t="n">
         <v>-1141.46</v>
@@ -1233,43 +1350,43 @@
         <v>-743.5</v>
       </c>
       <c r="E3" t="n">
-        <v>-620.6500000000001</v>
+        <v>-651.6500000000001</v>
       </c>
       <c r="F3" t="n">
-        <v>-335.1400000000001</v>
+        <v>-316.1400000000001</v>
       </c>
       <c r="G3" t="n">
-        <v>27.27000000000005</v>
+        <v>69.27000000000005</v>
       </c>
       <c r="H3" t="n">
-        <v>193.87</v>
+        <v>254.87</v>
       </c>
       <c r="I3" t="n">
-        <v>379.3449999999998</v>
+        <v>454.3449999999998</v>
       </c>
       <c r="J3" t="n">
-        <v>534.7799999999999</v>
+        <v>618.7799999999999</v>
       </c>
       <c r="K3" t="n">
-        <v>483.6749999999999</v>
+        <v>570.675</v>
       </c>
       <c r="L3" t="n">
-        <v>452.2999999999998</v>
+        <v>538.2999999999998</v>
       </c>
       <c r="M3" t="n">
-        <v>367.57</v>
+        <v>445.57</v>
       </c>
       <c r="N3" t="n">
-        <v>149.0700000000001</v>
+        <v>215.0700000000001</v>
       </c>
       <c r="O3" t="n">
-        <v>-161.885</v>
+        <v>-112.885</v>
       </c>
       <c r="P3" t="n">
-        <v>-461.76</v>
+        <v>-434.76</v>
       </c>
       <c r="Q3" t="n">
-        <v>-820.285</v>
+        <v>-847.285</v>
       </c>
       <c r="R3" t="n">
         <v>-932.5600000000001</v>
@@ -1310,43 +1427,43 @@
         <v>-1021.5</v>
       </c>
       <c r="E4" t="n">
-        <v>-966.9799999999999</v>
+        <v>-1001.98</v>
       </c>
       <c r="F4" t="n">
-        <v>-861.235</v>
+        <v>-856.235</v>
       </c>
       <c r="G4" t="n">
-        <v>-428.7049999999999</v>
+        <v>-396.7049999999999</v>
       </c>
       <c r="H4" t="n">
-        <v>-144.71</v>
+        <v>-85.70999999999998</v>
       </c>
       <c r="I4" t="n">
-        <v>96.98000000000013</v>
+        <v>172.9800000000001</v>
       </c>
       <c r="J4" t="n">
-        <v>278.04</v>
+        <v>364.04</v>
       </c>
       <c r="K4" t="n">
-        <v>230.71</v>
+        <v>320.71</v>
       </c>
       <c r="L4" t="n">
-        <v>187.8149999999999</v>
+        <v>275.8149999999999</v>
       </c>
       <c r="M4" t="n">
-        <v>79.84499999999994</v>
+        <v>158.8449999999999</v>
       </c>
       <c r="N4" t="n">
-        <v>-180.765</v>
+        <v>-115.765</v>
       </c>
       <c r="O4" t="n">
-        <v>-573.1600000000001</v>
+        <v>-530.1600000000001</v>
       </c>
       <c r="P4" t="n">
-        <v>-991.62</v>
+        <v>-976.62</v>
       </c>
       <c r="Q4" t="n">
-        <v>-1263.34</v>
+        <v>-1298.34</v>
       </c>
       <c r="R4" t="n">
         <v>-1258.22</v>
@@ -1486,34 +1603,34 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>681.5910000000275</v>
+        <v>683.8020000000275</v>
       </c>
       <c r="H2" t="n">
-        <v>1912.524000000063</v>
+        <v>1918.728000000063</v>
       </c>
       <c r="I2" t="n">
-        <v>3153.630000000094</v>
+        <v>3163.860000000123</v>
       </c>
       <c r="J2" t="n">
-        <v>3926.778000000103</v>
+        <v>3939.516000000103</v>
       </c>
       <c r="K2" t="n">
-        <v>4038.68100000009</v>
+        <v>4051.78200000009</v>
       </c>
       <c r="L2" t="n">
-        <v>3560.55</v>
+        <v>3572.1</v>
       </c>
       <c r="M2" t="n">
-        <v>2675.499000000122</v>
+        <v>2684.178000000122</v>
       </c>
       <c r="N2" t="n">
-        <v>1607.334000000046</v>
+        <v>1612.548000001704</v>
       </c>
       <c r="O2" t="n">
-        <v>640.8990000000266</v>
+        <v>642.9780000000266</v>
       </c>
       <c r="P2" t="n">
-        <v>20.3460000000009</v>
+        <v>20.41200000000089</v>
       </c>
       <c r="Q2" t="n">
         <v>0</v>
@@ -1557,10 +1674,10 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>305.1900000000139</v>
+        <v>306.1800000000066</v>
       </c>
       <c r="F3" t="n">
-        <v>1586.988000000005</v>
+        <v>462</v>
       </c>
       <c r="G3" t="n">
         <v>504</v>
@@ -1569,19 +1686,19 @@
         <v>630</v>
       </c>
       <c r="I3" t="n">
-        <v>5969.8</v>
+        <v>646.8</v>
       </c>
       <c r="J3" t="n">
-        <v>2801.011999999985</v>
+        <v>672</v>
       </c>
       <c r="K3" t="n">
-        <v>798</v>
+        <v>6097</v>
       </c>
       <c r="L3" t="n">
-        <v>3750.747984894617</v>
+        <v>1785.794306701995</v>
       </c>
       <c r="M3" t="n">
-        <v>756</v>
+        <v>6055</v>
       </c>
       <c r="N3" t="n">
         <v>756</v>
@@ -1593,10 +1710,10 @@
         <v>672</v>
       </c>
       <c r="Q3" t="n">
-        <v>600.2070000000257</v>
+        <v>602.1540000000111</v>
       </c>
       <c r="R3" t="n">
-        <v>40.69200000000179</v>
+        <v>40.82400000000099</v>
       </c>
       <c r="S3" t="n">
         <v>0</v>
@@ -1637,37 +1754,37 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>457.7849999994903</v>
+        <v>459.2700000000117</v>
       </c>
       <c r="G4" t="n">
-        <v>677.8799999996648</v>
+        <v>677.88</v>
       </c>
       <c r="H4" t="n">
-        <v>805.5600000007973</v>
+        <v>4898.879999999999</v>
       </c>
       <c r="I4" t="n">
-        <v>6147.040000000002</v>
+        <v>824.04</v>
       </c>
       <c r="J4" t="n">
-        <v>2706.256266196849</v>
+        <v>6149.920000000035</v>
       </c>
       <c r="K4" t="n">
         <v>978.6</v>
       </c>
       <c r="L4" t="n">
-        <v>6303.280000000002</v>
+        <v>3894.396000000002</v>
       </c>
       <c r="M4" t="n">
-        <v>5643.37500000048</v>
+        <v>1282.178808080811</v>
       </c>
       <c r="N4" t="n">
-        <v>940.8</v>
+        <v>5419.386</v>
       </c>
       <c r="O4" t="n">
-        <v>925.6800000000574</v>
+        <v>925.6800000000001</v>
       </c>
       <c r="P4" t="n">
-        <v>1018.259999999893</v>
+        <v>1018.26</v>
       </c>
       <c r="Q4" t="n">
         <v>0</v>
@@ -1798,7 +1915,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>-5.384208634495735e-08</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -1813,25 +1930,25 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>1136.744000000566</v>
+        <v>1165.948000000503</v>
       </c>
       <c r="I2" t="n">
-        <v>2586.960000003307</v>
+        <v>2635.19</v>
       </c>
       <c r="J2" t="n">
-        <v>3536.198000000803</v>
+        <v>3595.936000000559</v>
       </c>
       <c r="K2" t="n">
-        <v>3570.375999999332</v>
+        <v>3631.477000000878</v>
       </c>
       <c r="L2" t="n">
-        <v>3000.680000001536</v>
+        <v>3055.23000000054</v>
       </c>
       <c r="M2" t="n">
-        <v>1975.874000003975</v>
+        <v>2016.553000002471</v>
       </c>
       <c r="N2" t="n">
-        <v>686.6240000014985</v>
+        <v>710.838000001704</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
@@ -1840,7 +1957,7 @@
         <v>0</v>
       </c>
       <c r="Q2" t="n">
-        <v>0</v>
+        <v>-1.257285475730896e-08</v>
       </c>
       <c r="R2" t="n">
         <v>0</v>
@@ -1861,7 +1978,7 @@
         <v>0</v>
       </c>
       <c r="X2" t="n">
-        <v>2.328306436538696e-09</v>
+        <v>0</v>
       </c>
       <c r="Y2" t="n">
         <v>0</v>
@@ -1884,7 +2001,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>1124.988000000005</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -1893,19 +2010,19 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>5323</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>2129.011999999985</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>5299</v>
       </c>
       <c r="L3" t="n">
-        <v>2952.747984894617</v>
+        <v>987.7943067019949</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>5299</v>
       </c>
       <c r="N3" t="n">
         <v>0</v>
@@ -1967,25 +2084,25 @@
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>4093.32</v>
       </c>
       <c r="I4" t="n">
-        <v>5323</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>1855.336266196784</v>
+        <v>5299</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>5323</v>
+        <v>2914.116000000002</v>
       </c>
       <c r="M4" t="n">
-        <v>4704.25500000048</v>
+        <v>343.0588080808104</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>4478.586</v>
       </c>
       <c r="O4" t="n">
         <v>0</v>
@@ -2006,7 +2123,7 @@
         <v>0</v>
       </c>
       <c r="U4" t="n">
-        <v>0</v>
+        <v>8.381903171539307e-09</v>
       </c>
       <c r="V4" t="n">
         <v>0</v>
@@ -2018,7 +2135,7 @@
         <v>0</v>
       </c>
       <c r="Y4" t="n">
-        <v>0</v>
+        <v>-3.841705620288849e-09</v>
       </c>
     </row>
   </sheetData>
@@ -2119,22 +2236,22 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1091.5</v>
+        <v>1211.510000000024</v>
       </c>
       <c r="C2" t="n">
-        <v>896.2599999486321</v>
+        <v>1016.25</v>
       </c>
       <c r="D2" t="n">
-        <v>941.8</v>
+        <v>1061.81</v>
       </c>
       <c r="E2" t="n">
-        <v>876.1599999999908</v>
+        <v>1031.169999999971</v>
       </c>
       <c r="F2" t="n">
-        <v>857.6200000002173</v>
+        <v>737.63</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>55.08300000175677</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -2158,37 +2275,37 @@
         <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>237.5459999969</v>
+        <v>307.6386772051288</v>
       </c>
       <c r="P2" t="n">
-        <v>1140.543999999999</v>
+        <v>900.4779999999982</v>
       </c>
       <c r="Q2" t="n">
-        <v>1156.31000000014</v>
+        <v>1071.299999990736</v>
       </c>
       <c r="R2" t="n">
-        <v>1141.460000000001</v>
+        <v>1141.460000000073</v>
       </c>
       <c r="S2" t="n">
-        <v>1144.01</v>
+        <v>1144.010000000071</v>
       </c>
       <c r="T2" t="n">
         <v>1049.76</v>
       </c>
       <c r="U2" t="n">
-        <v>1379.2</v>
+        <v>1139.2</v>
       </c>
       <c r="V2" t="n">
-        <v>1110.496225615265</v>
+        <v>1346.75</v>
       </c>
       <c r="W2" t="n">
-        <v>1297.99</v>
+        <v>1057.99</v>
       </c>
       <c r="X2" t="n">
-        <v>900.1300000023284</v>
+        <v>1140.130000000067</v>
       </c>
       <c r="Y2" t="n">
-        <v>944.45</v>
+        <v>1064.460000000069</v>
       </c>
     </row>
     <row r="3">
@@ -2199,13 +2316,13 @@
         <v>879.3</v>
       </c>
       <c r="C3" t="n">
-        <v>811.000000001378</v>
+        <v>811</v>
       </c>
       <c r="D3" t="n">
-        <v>743.4999999988978</v>
+        <v>743.5</v>
       </c>
       <c r="E3" t="n">
-        <v>315.4599999966101</v>
+        <v>345.4700000000003</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -2241,10 +2358,10 @@
         <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>220.0779999986006</v>
+        <v>245.1309999986256</v>
       </c>
       <c r="R3" t="n">
-        <v>891.8679999999982</v>
+        <v>891.7359999999999</v>
       </c>
       <c r="S3" t="n">
         <v>950.8</v>
@@ -2276,16 +2393,16 @@
         <v>1150.35</v>
       </c>
       <c r="C4" t="n">
-        <v>1086.22</v>
+        <v>1086.220000000058</v>
       </c>
       <c r="D4" t="n">
         <v>1021.5</v>
       </c>
       <c r="E4" t="n">
-        <v>966.9799999999973</v>
+        <v>1001.979999999997</v>
       </c>
       <c r="F4" t="n">
-        <v>403.45</v>
+        <v>396.965</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -2318,10 +2435,10 @@
         <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>1263.34</v>
+        <v>1298.339999999624</v>
       </c>
       <c r="R4" t="n">
-        <v>1258.22</v>
+        <v>1258.219999999972</v>
       </c>
       <c r="S4" t="n">
         <v>1269.11</v>
@@ -2330,19 +2447,19 @@
         <v>1424.59</v>
       </c>
       <c r="U4" t="n">
-        <v>1520.98</v>
+        <v>1520.980000008382</v>
       </c>
       <c r="V4" t="n">
-        <v>1498.26</v>
+        <v>1494.3</v>
       </c>
       <c r="W4" t="n">
         <v>1456.45</v>
       </c>
       <c r="X4" t="n">
-        <v>1306.929999999997</v>
+        <v>1306.930000000075</v>
       </c>
       <c r="Y4" t="n">
-        <v>1236.82</v>
+        <v>1101.296999999456</v>
       </c>
     </row>
   </sheetData>
@@ -2443,76 +2560,76 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>7866.319191918572</v>
+        <v>8180.556565658894</v>
       </c>
       <c r="C2" t="n">
-        <v>6961.006060606524</v>
+        <v>7154.041414143771</v>
       </c>
       <c r="D2" t="n">
-        <v>6009.692929293387</v>
+        <v>6081.506060608417</v>
       </c>
       <c r="E2" t="n">
-        <v>5124.682828283299</v>
+        <v>5039.920202022558</v>
       </c>
       <c r="F2" t="n">
-        <v>4258.4</v>
+        <v>4294.83939394175</v>
       </c>
       <c r="G2" t="n">
-        <v>4258.4</v>
+        <v>4239.2</v>
       </c>
       <c r="H2" t="n">
-        <v>5383.776560000812</v>
+        <v>5393.488520000497</v>
       </c>
       <c r="I2" t="n">
-        <v>7944.866960004087</v>
+        <v>8002.326620000496</v>
       </c>
       <c r="J2" t="n">
-        <v>11445.70298000488</v>
+        <v>11562.30326000105</v>
       </c>
       <c r="K2" t="n">
-        <v>14980.37522000566</v>
+        <v>15157.46549000192</v>
       </c>
       <c r="L2" t="n">
-        <v>17951.04842000718</v>
+        <v>18182.14319000245</v>
       </c>
       <c r="M2" t="n">
-        <v>19907.16368001112</v>
+        <v>20178.5306600049</v>
       </c>
       <c r="N2" t="n">
-        <v>20586.9214400126</v>
+        <v>20882.2602800056</v>
       </c>
       <c r="O2" t="n">
-        <v>20346.97598547028</v>
+        <v>20571.51414141513</v>
       </c>
       <c r="P2" t="n">
-        <v>19194.91133900563</v>
+        <v>19661.94040404139</v>
       </c>
       <c r="Q2" t="n">
-        <v>18026.92144001559</v>
+        <v>18579.81919192042</v>
       </c>
       <c r="R2" t="n">
-        <v>16873.93154102569</v>
+        <v>17426.82929293045</v>
       </c>
       <c r="S2" t="n">
-        <v>15718.36588446004</v>
+        <v>16271.26363636472</v>
       </c>
       <c r="T2" t="n">
-        <v>14658.0022480964</v>
+        <v>15210.90000000109</v>
       </c>
       <c r="U2" t="n">
-        <v>13264.87093496496</v>
+        <v>14060.19292929402</v>
       </c>
       <c r="V2" t="n">
-        <v>12143.15757575762</v>
+        <v>12699.83939394188</v>
       </c>
       <c r="W2" t="n">
-        <v>10832.05656565661</v>
+        <v>11631.16262626512</v>
       </c>
       <c r="X2" t="n">
-        <v>9922.834343434341</v>
+        <v>10479.51616161858</v>
       </c>
       <c r="Y2" t="n">
-        <v>8968.844444444445</v>
+        <v>9404.304040406392</v>
       </c>
     </row>
     <row r="3">
@@ -2520,76 +2637,76 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>6147.248484845339</v>
+        <v>6159.161616161615</v>
       </c>
       <c r="C3" t="n">
-        <v>5328.056565652028</v>
+        <v>5339.969696969697</v>
       </c>
       <c r="D3" t="n">
-        <v>4577.04646464304</v>
+        <v>4588.959595959596</v>
       </c>
       <c r="E3" t="n">
-        <v>4258.4</v>
+        <v>4240</v>
       </c>
       <c r="F3" t="n">
-        <v>5372.138120000014</v>
+        <v>4240</v>
       </c>
       <c r="G3" t="n">
-        <v>5372.138120000014</v>
+        <v>4240</v>
       </c>
       <c r="H3" t="n">
-        <v>5372.138120000117</v>
+        <v>4240</v>
       </c>
       <c r="I3" t="n">
-        <v>10641.90812000001</v>
+        <v>4240</v>
       </c>
       <c r="J3" t="n">
-        <v>12749.63</v>
+        <v>4240</v>
       </c>
       <c r="K3" t="n">
-        <v>12749.63</v>
+        <v>9486.009999999729</v>
       </c>
       <c r="L3" t="n">
-        <v>15672.85050504567</v>
+        <v>10463.92636363498</v>
       </c>
       <c r="M3" t="n">
-        <v>15672.85050504567</v>
+        <v>15709.93636363498</v>
       </c>
       <c r="N3" t="n">
-        <v>15672.85050504567</v>
+        <v>15709.93636363498</v>
       </c>
       <c r="O3" t="n">
-        <v>15672.85050504567</v>
+        <v>15709.93636363498</v>
       </c>
       <c r="P3" t="n">
-        <v>15672.85050504567</v>
+        <v>15709.93636363498</v>
       </c>
       <c r="Q3" t="n">
-        <v>15450.54949494608</v>
+        <v>15462.32929292929</v>
       </c>
       <c r="R3" t="n">
-        <v>14549.67272726931</v>
+        <v>14561.58585858586</v>
       </c>
       <c r="S3" t="n">
-        <v>13589.26868686528</v>
+        <v>13601.18181818182</v>
       </c>
       <c r="T3" t="n">
-        <v>12474.62222221882</v>
+        <v>12486.53535353486</v>
       </c>
       <c r="U3" t="n">
-        <v>11264.01616161301</v>
+        <v>11275.9292929288</v>
       </c>
       <c r="V3" t="n">
-        <v>10079.16767676453</v>
+        <v>10091.08080808081</v>
       </c>
       <c r="W3" t="n">
-        <v>8937.955555552406</v>
+        <v>8949.868686868538</v>
       </c>
       <c r="X3" t="n">
-        <v>7950.58181817867</v>
+        <v>7962.494949494516</v>
       </c>
       <c r="Y3" t="n">
-        <v>7035.430303027157</v>
+        <v>7047.343434343433</v>
       </c>
     </row>
     <row r="4">
@@ -2597,76 +2714,76 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>7771.682828282733</v>
+        <v>7781.285858585858</v>
       </c>
       <c r="C4" t="n">
-        <v>6674.490909090813</v>
+        <v>6684.093939393937</v>
       </c>
       <c r="D4" t="n">
-        <v>5642.67272727324</v>
+        <v>5652.275757575755</v>
       </c>
       <c r="E4" t="n">
-        <v>4665.925252525767</v>
+        <v>4640.174747474747</v>
       </c>
       <c r="F4" t="n">
-        <v>4258.4</v>
+        <v>4239.2</v>
       </c>
       <c r="G4" t="n">
-        <v>4258.4</v>
+        <v>4239.2</v>
       </c>
       <c r="H4" t="n">
-        <v>4258.4</v>
+        <v>8291.586799999999</v>
       </c>
       <c r="I4" t="n">
-        <v>9528.17000000046</v>
+        <v>8291.586799999999</v>
       </c>
       <c r="J4" t="n">
-        <v>11364.95290353488</v>
+        <v>13537.59679999979</v>
       </c>
       <c r="K4" t="n">
-        <v>11364.95290353488</v>
+        <v>13537.5968</v>
       </c>
       <c r="L4" t="n">
-        <v>16634.72290353488</v>
+        <v>16422.57164</v>
       </c>
       <c r="M4" t="n">
-        <v>21291.93535353536</v>
+        <v>16762.19986</v>
       </c>
       <c r="N4" t="n">
-        <v>21291.93535353536</v>
+        <v>21196</v>
       </c>
       <c r="O4" t="n">
-        <v>21291.93535353536</v>
+        <v>21196</v>
       </c>
       <c r="P4" t="n">
-        <v>21291.93535353525</v>
+        <v>21196</v>
       </c>
       <c r="Q4" t="n">
-        <v>20015.83434343424</v>
+        <v>19884.54545454584</v>
       </c>
       <c r="R4" t="n">
-        <v>18744.90505050495</v>
+        <v>18613.61616161637</v>
       </c>
       <c r="S4" t="n">
-        <v>17462.97575757566</v>
+        <v>17331.68686868708</v>
       </c>
       <c r="T4" t="n">
-        <v>16023.99595959586</v>
+        <v>15892.70707070728</v>
       </c>
       <c r="U4" t="n">
-        <v>14487.65252525243</v>
+        <v>14356.36363636368</v>
       </c>
       <c r="V4" t="n">
-        <v>12974.25858585849</v>
+        <v>12846.96969696969</v>
       </c>
       <c r="W4" t="n">
-        <v>11503.09696969687</v>
+        <v>11375.80808080808</v>
       </c>
       <c r="X4" t="n">
-        <v>10182.96565656556</v>
+        <v>10055.67676767669</v>
       </c>
       <c r="Y4" t="n">
-        <v>8933.65252525243</v>
+        <v>8943.255555555555</v>
       </c>
     </row>
     <row r="5">
@@ -6352,13 +6469,13 @@
         <v>311.1</v>
       </c>
       <c r="K2" t="n">
-        <v>349.0950000006674</v>
+        <v>349.095000000787</v>
       </c>
       <c r="L2" t="n">
         <v>268.7700000011828</v>
       </c>
       <c r="M2" t="n">
-        <v>116.5350000018088</v>
+        <v>116.5350000022445</v>
       </c>
       <c r="N2" t="n">
         <v>0</v>
@@ -6685,7 +6802,7 @@
         <v>84.32000000204425</v>
       </c>
       <c r="N2" t="n">
-        <v>42.56000000145286</v>
+        <v>42.56000000000001</v>
       </c>
       <c r="O2" t="n">
         <v>4.800000003073364</v>
@@ -6735,7 +6852,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>2.00000000337088</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -6771,7 +6888,7 @@
         <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>11.6000000013737</v>
+        <v>11.60000000136327</v>
       </c>
       <c r="R3" t="n">
         <v>0</v>
@@ -6886,7 +7003,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6895,30 +7012,77 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Total Revenues</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Total Capital Costs</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Total Operation Variable Costs</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Total Operation Fixed Costs</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Total Profits</t>
-        </is>
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="2">
@@ -6926,19 +7090,230 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>3375173.553962285</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>4111500</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>427018.4369220809</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>187210</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>-1350554.882959796</v>
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>7.999999996707519</v>
+      </c>
+      <c r="H2" t="n">
+        <v>23</v>
+      </c>
+      <c r="I2" t="n">
+        <v>38</v>
+      </c>
+      <c r="J2" t="n">
+        <v>47</v>
+      </c>
+      <c r="K2" t="n">
+        <v>48</v>
+      </c>
+      <c r="L2" t="n">
+        <v>43</v>
+      </c>
+      <c r="M2" t="n">
+        <v>31.99999999806004</v>
+      </c>
+      <c r="N2" t="n">
+        <v>19</v>
+      </c>
+      <c r="O2" t="n">
+        <v>7</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>5</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>